<commit_message>
Added dimensions on relays to aggregation
See Excel Sheet 3
</commit_message>
<xml_diff>
--- a/visOgram.xlsx
+++ b/visOgram.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="0" windowWidth="21580" windowHeight="21920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="20580" windowHeight="22560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="202">
   <si>
     <t>RELAY</t>
   </si>
@@ -563,6 +564,69 @@
   </si>
   <si>
     <t>stuff are</t>
+  </si>
+  <si>
+    <t>as_spread</t>
+  </si>
+  <si>
+    <t>osv_r_nodes</t>
+  </si>
+  <si>
+    <t>osv_r_bwa</t>
+  </si>
+  <si>
+    <t>osv_r_bwc</t>
+  </si>
+  <si>
+    <t>osv_r_pbr</t>
+  </si>
+  <si>
+    <t>tsv_r_nodes</t>
+  </si>
+  <si>
+    <t>tsv_r_bwa</t>
+  </si>
+  <si>
+    <t>tsv_r_bwc</t>
+  </si>
+  <si>
+    <t>tsv_r_pbr</t>
+  </si>
+  <si>
+    <t>fast_r_nodes</t>
+  </si>
+  <si>
+    <t>fast_r_bwa</t>
+  </si>
+  <si>
+    <t>fast_r_bwc</t>
+  </si>
+  <si>
+    <t>fast_r_pbr</t>
+  </si>
+  <si>
+    <t>stable_r_nodes</t>
+  </si>
+  <si>
+    <t>stable_r_bwa</t>
+  </si>
+  <si>
+    <t>stable_r_bwc</t>
+  </si>
+  <si>
+    <t>stable_r_pbr</t>
+  </si>
+  <si>
+    <t>as_r_nodes</t>
+  </si>
+  <si>
+    <t>as_r_bwa</t>
+  </si>
+  <si>
+    <t>as_r_bwc</t>
+  </si>
+  <si>
+    <t>as_r_pbr</t>
   </si>
 </sst>
 </file>
@@ -608,7 +672,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,6 +835,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -781,7 +857,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -905,8 +981,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -940,8 +1046,10 @@
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="153">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1003,6 +1111,21 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1064,6 +1187,21 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2174,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2875,72 +3013,72 @@
       <c r="I43" s="3"/>
     </row>
     <row r="44" spans="2:11">
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G44" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" s="14"/>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="C45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="2" t="s">
+      <c r="E45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H45" s="3"/>
+      <c r="I45" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K45" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11">
-      <c r="C45" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G45" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="H45" s="14"/>
-      <c r="K45" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="46" spans="2:11">
       <c r="C46" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" s="14"/>
+      <c r="K46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="C47" s="12" t="s">
         <v>163</v>
-      </c>
-      <c r="D46" t="s">
-        <v>53</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H46" s="14"/>
-    </row>
-    <row r="47" spans="2:11">
-      <c r="C47" t="s">
-        <v>20</v>
       </c>
       <c r="D47" t="s">
         <v>53</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G47" s="23" t="s">
-        <v>80</v>
+        <v>5</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="H47" s="14"/>
     </row>
@@ -3340,7 +3478,7 @@
     </row>
     <row r="73" spans="2:9">
       <c r="C73" s="25" t="s">
-        <v>19</v>
+        <v>181</v>
       </c>
       <c r="D73" t="s">
         <v>81</v>
@@ -3680,7 +3818,7 @@
     </row>
     <row r="99" spans="3:8">
       <c r="C99" s="28"/>
-      <c r="D99" s="3" t="s">
+      <c r="D99" s="12" t="s">
         <v>20</v>
       </c>
       <c r="F99" s="3" t="s">
@@ -3698,6 +3836,1670 @@
       <c r="F100" s="28"/>
       <c r="G100" s="28"/>
       <c r="H100" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J124"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="11" customFormat="1">
+      <c r="A1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="B18" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="B19" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="F19" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="B20" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="F20" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="F21" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="B23" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="B24" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="B25" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="B34" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="B36" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="B38" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="B40" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="B41" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G44" s="14"/>
+      <c r="H44" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="B45" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="14"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="B46" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="14"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47" s="14"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="B48" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="14"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="B49" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G49" s="14"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="B51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="B52" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G52" s="14"/>
+      <c r="H52" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="B53" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G53" s="14"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="B54" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G54" s="14"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="B55" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" s="14"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="B56" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" s="14"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="B57" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G57" s="14"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="B59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G59" s="3"/>
+      <c r="H59" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="B60" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60" s="14"/>
+      <c r="H60" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="B61" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G61" s="14"/>
+      <c r="H61" s="3"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="B62" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="3"/>
+      <c r="F62" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G62" s="14"/>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="B63" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G63" s="14"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="B64" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G64" s="14"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="B65" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F65" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G65" s="14"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="B66" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G66" s="14"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="B67" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" t="s">
+        <v>53</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F67" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G67" s="14"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="B69" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G69" s="3"/>
+      <c r="H69" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="B70" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C70" t="s">
+        <v>81</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F70" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G70" s="14"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="B71" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C71" t="s">
+        <v>53</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G71" s="14"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="B73" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" t="s">
+        <v>54</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G73" s="3"/>
+      <c r="I73" t="s">
+        <v>109</v>
+      </c>
+      <c r="J73" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="B74" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G74" s="14"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="B75" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E75" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G75" s="14"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="B76" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" t="s">
+        <v>59</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="B77" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G77" s="14"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="B78" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C78" t="s">
+        <v>81</v>
+      </c>
+      <c r="E78" t="s">
+        <v>39</v>
+      </c>
+      <c r="F78" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G78" s="14"/>
+      <c r="H78" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="I78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="B79" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C79" t="s">
+        <v>54</v>
+      </c>
+      <c r="E79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G79" s="14"/>
+      <c r="H79" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I79" t="s">
+        <v>25</v>
+      </c>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="B80" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C80" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80" t="s">
+        <v>40</v>
+      </c>
+      <c r="F80" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G80" s="3"/>
+      <c r="H80" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="B82" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C82" t="s">
+        <v>52</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+      <c r="I82" t="s">
+        <v>109</v>
+      </c>
+      <c r="J82" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="B83" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" t="s">
+        <v>52</v>
+      </c>
+      <c r="D83" t="s">
+        <v>5</v>
+      </c>
+      <c r="J83" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="B84" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" t="s">
+        <v>52</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5</v>
+      </c>
+      <c r="J84" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="B85" t="s">
+        <v>97</v>
+      </c>
+      <c r="C85" t="s">
+        <v>53</v>
+      </c>
+      <c r="E85" t="s">
+        <v>41</v>
+      </c>
+      <c r="F85" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I85" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="B86" t="s">
+        <v>98</v>
+      </c>
+      <c r="C86" t="s">
+        <v>53</v>
+      </c>
+      <c r="E86" t="s">
+        <v>40</v>
+      </c>
+      <c r="I86" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="B88" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C88" t="s">
+        <v>59</v>
+      </c>
+      <c r="E88" t="s">
+        <v>48</v>
+      </c>
+      <c r="F88" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="B89" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C89" t="s">
+        <v>59</v>
+      </c>
+      <c r="E89" t="s">
+        <v>48</v>
+      </c>
+      <c r="F89" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="B90" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C90" t="s">
+        <v>59</v>
+      </c>
+      <c r="E90" t="s">
+        <v>48</v>
+      </c>
+      <c r="F90" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="B91" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C91" t="s">
+        <v>59</v>
+      </c>
+      <c r="E91" t="s">
+        <v>48</v>
+      </c>
+      <c r="F91" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="B92" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E92" t="s">
+        <v>48</v>
+      </c>
+      <c r="F92" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="B93" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E93" t="s">
+        <v>48</v>
+      </c>
+      <c r="F93" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H93" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="B94" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E94" t="s">
+        <v>48</v>
+      </c>
+      <c r="F94" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H94" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="B95" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E95" t="s">
+        <v>48</v>
+      </c>
+      <c r="F95" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="B96" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E96" t="s">
+        <v>48</v>
+      </c>
+      <c r="F96" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H96" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="B97" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C97" t="s">
+        <v>81</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F97" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H97" s="9"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="B98" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C98" t="s">
+        <v>59</v>
+      </c>
+      <c r="E98" t="s">
+        <v>48</v>
+      </c>
+      <c r="F98" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H98" s="9"/>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="B99" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C99" t="s">
+        <v>59</v>
+      </c>
+      <c r="E99" t="s">
+        <v>48</v>
+      </c>
+      <c r="F99" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H99" s="9"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="B100" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C100" t="s">
+        <v>52</v>
+      </c>
+      <c r="E100" t="s">
+        <v>48</v>
+      </c>
+      <c r="F100" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H100" s="9"/>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="B101" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C101" t="s">
+        <v>52</v>
+      </c>
+      <c r="E101" t="s">
+        <v>48</v>
+      </c>
+      <c r="F101" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H101" s="9"/>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="B103" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" t="s">
+        <v>147</v>
+      </c>
+      <c r="F103" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="B104" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="B105" s="28"/>
+      <c r="C105" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G105" s="28"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="B106" s="28"/>
+      <c r="C106" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G106" s="28"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="B107" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G107" s="28"/>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="B108" s="28"/>
+      <c r="C108" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E108" t="s">
+        <v>48</v>
+      </c>
+      <c r="F108" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G108" s="28"/>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="B109" s="28"/>
+      <c r="C109" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
+        <v>48</v>
+      </c>
+      <c r="F109" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G109" s="28"/>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="B110" s="28"/>
+      <c r="C110" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G110" s="28"/>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="B111" s="28"/>
+      <c r="C111" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G111" s="28"/>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="B112" s="28"/>
+      <c r="C112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G112" s="28"/>
+    </row>
+    <row r="113" spans="2:7">
+      <c r="B113" s="28"/>
+      <c r="C113" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G113" s="28"/>
+    </row>
+    <row r="114" spans="2:7">
+      <c r="B114" s="28"/>
+      <c r="C114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G114" s="28"/>
+    </row>
+    <row r="115" spans="2:7">
+      <c r="B115" s="28"/>
+      <c r="C115" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G115" s="28"/>
+    </row>
+    <row r="116" spans="2:7">
+      <c r="B116" s="28"/>
+      <c r="C116" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G116" s="28"/>
+    </row>
+    <row r="117" spans="2:7">
+      <c r="B117" s="28"/>
+      <c r="C117" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G117" s="28"/>
+    </row>
+    <row r="118" spans="2:7">
+      <c r="B118" s="28"/>
+      <c r="C118" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G118" s="28"/>
+    </row>
+    <row r="119" spans="2:7">
+      <c r="B119" s="28"/>
+      <c r="C119" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G119" s="28"/>
+    </row>
+    <row r="120" spans="2:7">
+      <c r="B120" s="28"/>
+      <c r="C120" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G120" s="28"/>
+    </row>
+    <row r="121" spans="2:7">
+      <c r="B121" s="28"/>
+      <c r="C121" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G121" s="28"/>
+    </row>
+    <row r="122" spans="2:7">
+      <c r="B122" s="28"/>
+      <c r="C122" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F122" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G122" s="28"/>
+    </row>
+    <row r="123" spans="2:7">
+      <c r="B123" s="28"/>
+      <c r="C123" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F123" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G123" s="28"/>
+    </row>
+    <row r="124" spans="2:7">
+      <c r="B124" s="28"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="28"/>
+      <c r="E124" s="28"/>
+      <c r="F124" s="28"/>
+      <c r="G124" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added comments from mailinglist
this is  just a first step to make sure essential parts from the mail
conversations aren't forgotten. the comments need to be weaved into the
text

some other rather minor changes
</commit_message>
<xml_diff>
--- a/visOgram.xlsx
+++ b/visOgram.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23880" windowHeight="23560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="18340" yWindow="0" windowWidth="17720" windowHeight="23560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="241">
   <si>
     <t>RELAY</t>
   </si>
@@ -718,6 +718,33 @@
   </si>
   <si>
     <t>TSV</t>
+  </si>
+  <si>
+    <t>directories could be split in directories with ad without authority flag</t>
+  </si>
+  <si>
+    <t>and if they were given out by email, http or other</t>
+  </si>
+  <si>
+    <t>and if they are located in the ec2 cloud</t>
+  </si>
+  <si>
+    <t>bridges could be split in pluggable transports obfs2, obfs3, both,none</t>
+  </si>
+  <si>
+    <t>which makes 4x3x2 = 24 permutations for bridges</t>
+  </si>
+  <si>
+    <t>every exit entry could be split up into the 3 exit port s permitted: 80, 443, 6667</t>
+  </si>
+  <si>
+    <t>filter out nodes below a certain bw treshold</t>
+  </si>
+  <si>
+    <t>how about guard+!badexit?</t>
+  </si>
+  <si>
+    <t>but how would we do that?</t>
   </si>
 </sst>
 </file>
@@ -5828,15 +5855,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="L107" sqref="L107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -5846,8 +5873,11 @@
       <c r="D1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="B2" t="s">
         <v>228</v>
       </c>
@@ -5855,15 +5885,18 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>148</v>
       </c>
       <c r="D3" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -5874,15 +5907,18 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>85</v>
       </c>
       <c r="D5" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="F5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>106</v>
       </c>
@@ -5890,39 +5926,51 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="F7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="F8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="F9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>88</v>
       </c>
       <c r="D10" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="F10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="14"/>
       <c r="B11" s="14" t="s">
         <v>93</v>
@@ -5932,7 +5980,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>215</v>
       </c>
@@ -5942,16 +5990,22 @@
       <c r="D12" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="F12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="C13" t="s">
         <v>106</v>
       </c>
       <c r="D13" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="C14" t="s">
         <v>11</v>
       </c>
@@ -5959,7 +6013,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="C15" t="s">
         <v>13</v>
       </c>
@@ -5967,7 +6021,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="B16" t="s">
         <v>216</v>
       </c>

</xml_diff>